<commit_message>
rdm all weighed and inputted
</commit_message>
<xml_diff>
--- a/rdm.gradient.2019.datasheet.xlsx
+++ b/rdm.gradient.2019.datasheet.xlsx
@@ -365,8 +365,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,8 +651,8 @@
   <dimension ref="A1:V635"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A190" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E192" sqref="E192"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A113" sqref="A113:XFD113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,6 +750,9 @@
       <c r="D2" t="s">
         <v>59</v>
       </c>
+      <c r="E2">
+        <v>9.9628999999999994</v>
+      </c>
       <c r="F2">
         <v>355</v>
       </c>
@@ -802,6 +806,9 @@
       <c r="D3" t="s">
         <v>20</v>
       </c>
+      <c r="E3">
+        <v>2.5404</v>
+      </c>
       <c r="I3">
         <v>15</v>
       </c>
@@ -837,6 +844,9 @@
       <c r="D4" t="s">
         <v>59</v>
       </c>
+      <c r="E4">
+        <v>5.7949000000000002</v>
+      </c>
       <c r="F4">
         <v>430</v>
       </c>
@@ -884,6 +894,9 @@
       <c r="D5" t="s">
         <v>20</v>
       </c>
+      <c r="E5">
+        <v>4.2241999999999997</v>
+      </c>
       <c r="I5">
         <v>1</v>
       </c>
@@ -919,6 +932,9 @@
       <c r="D6" t="s">
         <v>59</v>
       </c>
+      <c r="E6">
+        <v>3.4054000000000002</v>
+      </c>
       <c r="F6">
         <v>520</v>
       </c>
@@ -1004,6 +1020,9 @@
       <c r="D8" t="s">
         <v>59</v>
       </c>
+      <c r="E8">
+        <v>1.7950999999999999</v>
+      </c>
       <c r="F8">
         <v>370</v>
       </c>
@@ -1051,6 +1070,9 @@
       <c r="D9" t="s">
         <v>20</v>
       </c>
+      <c r="E9">
+        <v>3.6812999999999998</v>
+      </c>
       <c r="I9">
         <v>0</v>
       </c>
@@ -1086,6 +1108,9 @@
       <c r="D10" t="s">
         <v>59</v>
       </c>
+      <c r="E10">
+        <v>4.2586000000000004</v>
+      </c>
       <c r="F10">
         <v>455</v>
       </c>
@@ -1133,6 +1158,9 @@
       <c r="D11" t="s">
         <v>20</v>
       </c>
+      <c r="E11">
+        <v>3.4074</v>
+      </c>
       <c r="I11">
         <v>0</v>
       </c>
@@ -1168,6 +1196,9 @@
       <c r="D12" t="s">
         <v>59</v>
       </c>
+      <c r="E12">
+        <v>2.5606</v>
+      </c>
       <c r="F12">
         <v>275</v>
       </c>
@@ -1224,6 +1255,9 @@
       <c r="D13" t="s">
         <v>20</v>
       </c>
+      <c r="E13">
+        <v>1.8807</v>
+      </c>
       <c r="I13">
         <v>7</v>
       </c>
@@ -1268,6 +1302,9 @@
       <c r="D14" t="s">
         <v>59</v>
       </c>
+      <c r="E14">
+        <v>2.9022999999999999</v>
+      </c>
       <c r="F14">
         <v>275</v>
       </c>
@@ -1315,6 +1352,9 @@
       <c r="D15" t="s">
         <v>20</v>
       </c>
+      <c r="E15">
+        <v>0.60829999999999995</v>
+      </c>
       <c r="I15">
         <v>5</v>
       </c>
@@ -1350,6 +1390,9 @@
       <c r="D16" t="s">
         <v>59</v>
       </c>
+      <c r="E16">
+        <v>5.9177</v>
+      </c>
       <c r="F16">
         <v>310</v>
       </c>
@@ -1406,6 +1449,9 @@
       <c r="D17" t="s">
         <v>20</v>
       </c>
+      <c r="E17">
+        <v>2.8927999999999998</v>
+      </c>
       <c r="I17">
         <v>0</v>
       </c>
@@ -1450,6 +1496,9 @@
       <c r="D18" t="s">
         <v>59</v>
       </c>
+      <c r="E18">
+        <v>4.4363999999999999</v>
+      </c>
       <c r="F18">
         <v>135</v>
       </c>
@@ -1497,6 +1546,9 @@
       <c r="D19" t="s">
         <v>20</v>
       </c>
+      <c r="E19">
+        <v>0.36</v>
+      </c>
       <c r="I19">
         <v>5</v>
       </c>
@@ -1814,6 +1866,9 @@
       <c r="D26" t="s">
         <v>59</v>
       </c>
+      <c r="E26">
+        <v>4.7470999999999997</v>
+      </c>
       <c r="F26">
         <v>175</v>
       </c>
@@ -1861,6 +1916,9 @@
       <c r="D27" t="s">
         <v>20</v>
       </c>
+      <c r="E27">
+        <v>1.8113999999999999</v>
+      </c>
       <c r="I27">
         <v>0</v>
       </c>
@@ -1896,6 +1954,9 @@
       <c r="D28" t="s">
         <v>59</v>
       </c>
+      <c r="E28">
+        <v>4.0217000000000001</v>
+      </c>
       <c r="F28">
         <v>530</v>
       </c>
@@ -1943,6 +2004,9 @@
       <c r="D29" t="s">
         <v>20</v>
       </c>
+      <c r="E29">
+        <v>1.1736</v>
+      </c>
       <c r="I29">
         <v>1</v>
       </c>
@@ -1978,6 +2042,9 @@
       <c r="D30" t="s">
         <v>59</v>
       </c>
+      <c r="E30">
+        <v>4.8583999999999996</v>
+      </c>
       <c r="F30">
         <v>565</v>
       </c>
@@ -2025,6 +2092,9 @@
       <c r="D31" t="s">
         <v>20</v>
       </c>
+      <c r="E31">
+        <v>2.6166</v>
+      </c>
       <c r="I31">
         <v>1</v>
       </c>
@@ -2060,6 +2130,9 @@
       <c r="D32" t="s">
         <v>59</v>
       </c>
+      <c r="E32">
+        <v>1.9785999999999999</v>
+      </c>
       <c r="F32">
         <v>580</v>
       </c>
@@ -2116,6 +2189,9 @@
       <c r="D33" t="s">
         <v>20</v>
       </c>
+      <c r="E33">
+        <v>4.6700999999999997</v>
+      </c>
       <c r="I33">
         <v>0</v>
       </c>
@@ -2160,6 +2236,9 @@
       <c r="D34" t="s">
         <v>59</v>
       </c>
+      <c r="E34">
+        <v>4.28</v>
+      </c>
       <c r="F34">
         <v>265</v>
       </c>
@@ -2207,6 +2286,9 @@
       <c r="D35" t="s">
         <v>20</v>
       </c>
+      <c r="E35">
+        <v>1.8539000000000001</v>
+      </c>
       <c r="I35">
         <v>2</v>
       </c>
@@ -5542,35 +5624,38 @@
         <v>87</v>
       </c>
     </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="113" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C113">
+      <c r="C113" s="1">
         <v>17</v>
       </c>
-      <c r="D113" t="s">
-        <v>20</v>
-      </c>
-      <c r="I113">
+      <c r="D113" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E113" s="1">
+        <v>0</v>
+      </c>
+      <c r="I113" s="1">
         <v>4</v>
       </c>
-      <c r="K113">
+      <c r="K113" s="1">
         <v>22</v>
       </c>
-      <c r="L113">
+      <c r="L113" s="1">
         <v>5</v>
       </c>
-      <c r="M113">
-        <v>0</v>
-      </c>
-      <c r="N113">
+      <c r="M113" s="1">
+        <v>0</v>
+      </c>
+      <c r="N113" s="1">
         <v>95</v>
       </c>
-      <c r="U113" t="s">
+      <c r="U113" s="1" t="s">
         <v>87</v>
       </c>
     </row>
@@ -5587,6 +5672,9 @@
       <c r="D114" t="s">
         <v>59</v>
       </c>
+      <c r="E114">
+        <v>5.1817000000000002</v>
+      </c>
       <c r="F114">
         <v>220</v>
       </c>
@@ -5666,6 +5754,9 @@
       <c r="D116" t="s">
         <v>59</v>
       </c>
+      <c r="E116">
+        <v>1.3083</v>
+      </c>
       <c r="F116">
         <v>270</v>
       </c>
@@ -5719,6 +5810,9 @@
       <c r="D117" t="s">
         <v>20</v>
       </c>
+      <c r="E117">
+        <v>1.6032</v>
+      </c>
       <c r="I117">
         <v>5</v>
       </c>
@@ -5807,6 +5901,9 @@
       <c r="D119" t="s">
         <v>20</v>
       </c>
+      <c r="E119">
+        <v>0.58460000000000001</v>
+      </c>
       <c r="I119">
         <v>2</v>
       </c>
@@ -7162,6 +7259,9 @@
       <c r="D150" t="s">
         <v>59</v>
       </c>
+      <c r="E150">
+        <v>2.3784000000000001</v>
+      </c>
       <c r="F150">
         <v>375</v>
       </c>
@@ -7215,6 +7315,9 @@
       <c r="D151" t="s">
         <v>20</v>
       </c>
+      <c r="E151">
+        <v>1.9238999999999999</v>
+      </c>
       <c r="I151">
         <v>0</v>
       </c>
@@ -7652,6 +7755,9 @@
       <c r="D161" t="s">
         <v>20</v>
       </c>
+      <c r="E161">
+        <v>1.1917</v>
+      </c>
       <c r="I161">
         <v>0</v>
       </c>
@@ -7684,6 +7790,9 @@
       <c r="D162" t="s">
         <v>59</v>
       </c>
+      <c r="E162">
+        <v>0.54759999999999998</v>
+      </c>
       <c r="F162">
         <v>230</v>
       </c>
@@ -7728,6 +7837,9 @@
       <c r="D163" t="s">
         <v>20</v>
       </c>
+      <c r="E163">
+        <v>0.58819999999999995</v>
+      </c>
       <c r="I163">
         <v>0</v>
       </c>
@@ -7760,6 +7872,9 @@
       <c r="D164" t="s">
         <v>59</v>
       </c>
+      <c r="E164">
+        <v>1.2768999999999999</v>
+      </c>
       <c r="F164">
         <v>280</v>
       </c>
@@ -7804,6 +7919,9 @@
       <c r="D165" t="s">
         <v>20</v>
       </c>
+      <c r="E165">
+        <v>5.0624000000000002</v>
+      </c>
       <c r="I165">
         <v>3</v>
       </c>
@@ -7836,6 +7954,9 @@
       <c r="D166" t="s">
         <v>59</v>
       </c>
+      <c r="E166">
+        <v>7.5600000000000001E-2</v>
+      </c>
       <c r="F166">
         <v>355</v>
       </c>
@@ -7880,6 +8001,9 @@
       <c r="D167" t="s">
         <v>20</v>
       </c>
+      <c r="E167">
+        <v>0.35110000000000002</v>
+      </c>
       <c r="I167">
         <v>0</v>
       </c>
@@ -7912,6 +8036,9 @@
       <c r="D168" t="s">
         <v>59</v>
       </c>
+      <c r="E168">
+        <v>2.0379</v>
+      </c>
       <c r="F168">
         <v>315</v>
       </c>
@@ -7968,6 +8095,9 @@
       <c r="D169" t="s">
         <v>20</v>
       </c>
+      <c r="E169">
+        <v>4.1589999999999998</v>
+      </c>
       <c r="I169">
         <v>2</v>
       </c>
@@ -8009,6 +8139,9 @@
       <c r="D170" t="s">
         <v>59</v>
       </c>
+      <c r="E170">
+        <v>3.5762</v>
+      </c>
       <c r="F170">
         <v>695</v>
       </c>
@@ -8056,6 +8189,9 @@
       <c r="D171" t="s">
         <v>20</v>
       </c>
+      <c r="E171">
+        <v>1.7867999999999999</v>
+      </c>
       <c r="I171">
         <v>1</v>
       </c>
@@ -8088,6 +8224,9 @@
       <c r="D172" t="s">
         <v>59</v>
       </c>
+      <c r="E172">
+        <v>5.5369999999999999</v>
+      </c>
       <c r="F172">
         <v>455</v>
       </c>
@@ -8236,147 +8375,153 @@
         <v>87</v>
       </c>
     </row>
-    <row r="176" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+    <row r="176" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B176" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C176">
+      <c r="C176" s="1">
         <v>26</v>
       </c>
-      <c r="D176" t="s">
+      <c r="D176" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F176">
+      <c r="E176" s="1">
+        <v>3.49</v>
+      </c>
+      <c r="F176" s="1">
         <v>290</v>
       </c>
-      <c r="G176">
+      <c r="G176" s="1">
         <v>240</v>
       </c>
-      <c r="H176">
+      <c r="H176" s="1">
         <v>125</v>
       </c>
-      <c r="I176">
+      <c r="I176" s="1">
         <v>3</v>
       </c>
-      <c r="J176">
+      <c r="J176" s="1">
         <v>3</v>
       </c>
-      <c r="K176">
+      <c r="K176" s="1">
         <v>37</v>
       </c>
-      <c r="L176">
+      <c r="L176" s="1">
         <v>35</v>
       </c>
-      <c r="M176">
-        <v>0</v>
-      </c>
-      <c r="N176">
+      <c r="M176" s="1">
+        <v>0</v>
+      </c>
+      <c r="N176" s="1">
         <v>65</v>
       </c>
-      <c r="R176" t="s">
+      <c r="R176" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S176" t="s">
+      <c r="S176" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="T176" t="s">
+      <c r="T176" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="U176" t="s">
+      <c r="U176" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="177" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+    <row r="177" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B177" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C177">
+      <c r="C177" s="1">
         <v>26</v>
       </c>
-      <c r="D177" t="s">
-        <v>20</v>
-      </c>
-      <c r="I177">
+      <c r="D177" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E177" s="1">
+        <v>0.94379999999999997</v>
+      </c>
+      <c r="I177" s="1">
         <v>4</v>
       </c>
-      <c r="K177">
+      <c r="K177" s="1">
         <v>22</v>
       </c>
-      <c r="L177">
+      <c r="L177" s="1">
         <v>15</v>
       </c>
-      <c r="M177">
-        <v>0</v>
-      </c>
-      <c r="N177">
+      <c r="M177" s="1">
+        <v>0</v>
+      </c>
+      <c r="N177" s="1">
         <v>85</v>
       </c>
-      <c r="R177" t="s">
+      <c r="R177" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S177" t="s">
+      <c r="S177" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="T177" t="s">
+      <c r="T177" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="U177" t="s">
+      <c r="U177" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="178" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
+    <row r="178" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B178" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C178">
+      <c r="C178" s="1">
         <v>27</v>
       </c>
-      <c r="D178" t="s">
+      <c r="D178" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E178">
-        <v>3.49</v>
-      </c>
-      <c r="F178">
+      <c r="E178" s="1">
+        <v>3.6248</v>
+      </c>
+      <c r="F178" s="1">
         <v>190</v>
       </c>
-      <c r="G178">
+      <c r="G178" s="1">
         <v>165</v>
       </c>
-      <c r="H178">
+      <c r="H178" s="1">
         <v>90</v>
       </c>
-      <c r="I178">
+      <c r="I178" s="1">
         <v>2</v>
       </c>
-      <c r="J178">
-        <v>0</v>
-      </c>
-      <c r="K178">
+      <c r="J178" s="1">
+        <v>0</v>
+      </c>
+      <c r="K178" s="1">
         <v>25</v>
       </c>
-      <c r="L178">
+      <c r="L178" s="1">
         <v>75</v>
       </c>
-      <c r="M178">
-        <v>0</v>
-      </c>
-      <c r="N178">
+      <c r="M178" s="1">
+        <v>0</v>
+      </c>
+      <c r="N178" s="1">
         <v>25</v>
       </c>
-      <c r="Q178" t="s">
+      <c r="Q178" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="U178" t="s">
+      <c r="U178" s="1" t="s">
         <v>87</v>
       </c>
     </row>
@@ -8393,6 +8538,9 @@
       <c r="D179" t="s">
         <v>20</v>
       </c>
+      <c r="E179">
+        <v>4.9684999999999997</v>
+      </c>
       <c r="I179">
         <v>3</v>
       </c>
@@ -8762,38 +8910,38 @@
         <v>91</v>
       </c>
     </row>
-    <row r="187" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+    <row r="187" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B187" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C187">
+      <c r="C187" s="1">
         <v>1</v>
       </c>
-      <c r="D187" t="s">
-        <v>20</v>
-      </c>
-      <c r="E187">
-        <v>3.7233999999999998</v>
-      </c>
-      <c r="I187">
-        <v>0</v>
-      </c>
-      <c r="K187">
+      <c r="D187" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E187" s="1">
+        <v>1.9574</v>
+      </c>
+      <c r="I187" s="1">
+        <v>0</v>
+      </c>
+      <c r="K187" s="1">
         <v>17</v>
       </c>
-      <c r="L187">
+      <c r="L187" s="1">
         <v>60</v>
       </c>
-      <c r="M187">
-        <v>0</v>
-      </c>
-      <c r="N187">
+      <c r="M187" s="1">
+        <v>0</v>
+      </c>
+      <c r="N187" s="1">
         <v>40</v>
       </c>
-      <c r="U187" t="s">
+      <c r="U187" s="1" t="s">
         <v>91</v>
       </c>
     </row>
@@ -8810,6 +8958,9 @@
       <c r="D188" t="s">
         <v>59</v>
       </c>
+      <c r="E188">
+        <v>2.5613000000000001</v>
+      </c>
       <c r="F188">
         <v>410</v>
       </c>
@@ -8866,6 +9017,9 @@
       <c r="D189" t="s">
         <v>20</v>
       </c>
+      <c r="E189">
+        <v>0.6139</v>
+      </c>
       <c r="I189">
         <v>1</v>
       </c>
@@ -8992,6 +9146,9 @@
       <c r="D192" t="s">
         <v>59</v>
       </c>
+      <c r="E192">
+        <v>5.2461000000000002</v>
+      </c>
       <c r="F192">
         <v>685</v>
       </c>
@@ -9036,6 +9193,9 @@
       <c r="D193" t="s">
         <v>20</v>
       </c>
+      <c r="E193">
+        <v>0.3916</v>
+      </c>
       <c r="I193">
         <v>4</v>
       </c>
@@ -9303,6 +9463,9 @@
       <c r="D199" t="s">
         <v>20</v>
       </c>
+      <c r="E199" s="1">
+        <v>3.7233999999999998</v>
+      </c>
       <c r="I199">
         <v>3</v>
       </c>
@@ -9605,6 +9768,9 @@
       <c r="D206" t="s">
         <v>59</v>
       </c>
+      <c r="E206">
+        <v>1.8272999999999999</v>
+      </c>
       <c r="F206">
         <v>575</v>
       </c>
@@ -9649,6 +9815,9 @@
       <c r="D207" t="s">
         <v>20</v>
       </c>
+      <c r="E207">
+        <v>0.57099999999999995</v>
+      </c>
       <c r="I207">
         <v>4</v>
       </c>
@@ -9728,6 +9897,9 @@
       <c r="D209" t="s">
         <v>20</v>
       </c>
+      <c r="E209">
+        <v>0.25569999999999998</v>
+      </c>
       <c r="I209">
         <v>1</v>
       </c>
@@ -9810,6 +9982,9 @@
       <c r="D211" t="s">
         <v>20</v>
       </c>
+      <c r="E211">
+        <v>0.9587</v>
+      </c>
       <c r="I211">
         <v>2</v>
       </c>
@@ -9901,6 +10076,9 @@
       <c r="D213" t="s">
         <v>20</v>
       </c>
+      <c r="E213">
+        <v>0.44330000000000003</v>
+      </c>
       <c r="I213">
         <v>1</v>
       </c>
@@ -9995,6 +10173,9 @@
       <c r="D215" t="s">
         <v>20</v>
       </c>
+      <c r="E215">
+        <v>1.131</v>
+      </c>
       <c r="I215">
         <v>1</v>
       </c>
@@ -10027,6 +10208,9 @@
       <c r="D216" t="s">
         <v>59</v>
       </c>
+      <c r="E216">
+        <v>0</v>
+      </c>
       <c r="F216">
         <v>315</v>
       </c>
@@ -10191,6 +10375,9 @@
       <c r="D220" t="s">
         <v>59</v>
       </c>
+      <c r="E220">
+        <v>0.2944</v>
+      </c>
       <c r="F220">
         <v>375</v>
       </c>
@@ -10244,6 +10431,9 @@
       <c r="D221" t="s">
         <v>20</v>
       </c>
+      <c r="E221">
+        <v>0.27339999999999998</v>
+      </c>
       <c r="I221">
         <v>0</v>
       </c>
@@ -10449,6 +10639,9 @@
       <c r="D226" t="s">
         <v>59</v>
       </c>
+      <c r="E226">
+        <v>0.66469999999999996</v>
+      </c>
       <c r="F226">
         <v>305</v>
       </c>
@@ -10508,6 +10701,9 @@
       <c r="D227" t="s">
         <v>20</v>
       </c>
+      <c r="E227">
+        <v>3.7783000000000002</v>
+      </c>
       <c r="I227">
         <v>2</v>
       </c>
@@ -10716,6 +10912,9 @@
       <c r="D232" t="s">
         <v>59</v>
       </c>
+      <c r="E232">
+        <v>0</v>
+      </c>
       <c r="F232">
         <v>320</v>
       </c>
@@ -10880,6 +11079,9 @@
       <c r="D236" t="s">
         <v>59</v>
       </c>
+      <c r="E236">
+        <v>1.6736</v>
+      </c>
       <c r="F236">
         <v>380</v>
       </c>
@@ -10936,6 +11138,9 @@
       <c r="D237" t="s">
         <v>20</v>
       </c>
+      <c r="E237">
+        <v>8.5927000000000007</v>
+      </c>
       <c r="I237">
         <v>3</v>
       </c>
@@ -11232,6 +11437,9 @@
       <c r="D244" t="s">
         <v>59</v>
       </c>
+      <c r="E244">
+        <v>0</v>
+      </c>
       <c r="F244">
         <v>425</v>
       </c>
@@ -11291,6 +11499,9 @@
       <c r="D245" t="s">
         <v>20</v>
       </c>
+      <c r="E245">
+        <v>1.6039000000000001</v>
+      </c>
       <c r="I245">
         <v>0</v>
       </c>
@@ -12819,6 +13030,9 @@
       <c r="D280" t="s">
         <v>59</v>
       </c>
+      <c r="E280">
+        <v>0.12709999999999999</v>
+      </c>
       <c r="F280">
         <v>530</v>
       </c>
@@ -12998,6 +13212,9 @@
       <c r="D284" t="s">
         <v>59</v>
       </c>
+      <c r="E284">
+        <v>6.9348000000000001</v>
+      </c>
       <c r="F284">
         <v>425</v>
       </c>
@@ -13045,6 +13262,9 @@
       <c r="D285" t="s">
         <v>20</v>
       </c>
+      <c r="E285">
+        <v>0.44009999999999999</v>
+      </c>
       <c r="I285">
         <v>1</v>
       </c>
@@ -13617,6 +13837,9 @@
       <c r="D298" t="s">
         <v>59</v>
       </c>
+      <c r="E298">
+        <v>3.7827000000000002</v>
+      </c>
       <c r="F298">
         <v>355</v>
       </c>
@@ -13699,6 +13922,9 @@
       <c r="D300" t="s">
         <v>59</v>
       </c>
+      <c r="E300">
+        <v>4.2096</v>
+      </c>
       <c r="F300">
         <v>480</v>
       </c>
@@ -14045,6 +14271,9 @@
       <c r="D308" t="s">
         <v>59</v>
       </c>
+      <c r="E308">
+        <v>1.143</v>
+      </c>
       <c r="F308">
         <v>310</v>
       </c>
@@ -14098,6 +14327,9 @@
       <c r="D309" t="s">
         <v>20</v>
       </c>
+      <c r="E309">
+        <v>1.4325000000000001</v>
+      </c>
       <c r="I309">
         <v>2</v>
       </c>
@@ -15274,6 +15506,9 @@
       <c r="D336" t="s">
         <v>59</v>
       </c>
+      <c r="E336">
+        <v>2.8092000000000001</v>
+      </c>
       <c r="F336">
         <v>295</v>
       </c>
@@ -15708,6 +15943,9 @@
       <c r="D346" t="s">
         <v>59</v>
       </c>
+      <c r="E346">
+        <v>2.8620000000000001</v>
+      </c>
       <c r="F346">
         <v>490</v>
       </c>
@@ -15790,6 +16028,9 @@
       <c r="D348" t="s">
         <v>59</v>
       </c>
+      <c r="E348">
+        <v>5.6561000000000003</v>
+      </c>
       <c r="F348">
         <v>220</v>
       </c>
@@ -15846,6 +16087,9 @@
       <c r="D349" t="s">
         <v>20</v>
       </c>
+      <c r="E349">
+        <v>15.1671</v>
+      </c>
       <c r="I349">
         <v>2</v>
       </c>
@@ -16136,6 +16380,9 @@
       <c r="D356" t="s">
         <v>59</v>
       </c>
+      <c r="E356">
+        <v>9.9199999999999997E-2</v>
+      </c>
       <c r="F356">
         <v>360</v>
       </c>
@@ -16388,6 +16635,9 @@
       <c r="D362" t="s">
         <v>59</v>
       </c>
+      <c r="E362">
+        <v>3.1970000000000001</v>
+      </c>
       <c r="F362">
         <v>375</v>
       </c>
@@ -16570,6 +16820,9 @@
       <c r="D366" t="s">
         <v>59</v>
       </c>
+      <c r="E366">
+        <v>2.4279000000000002</v>
+      </c>
       <c r="F366">
         <v>160</v>
       </c>
@@ -16902,6 +17155,9 @@
       <c r="D373" t="s">
         <v>71</v>
       </c>
+      <c r="E373">
+        <v>1.2452000000000001</v>
+      </c>
       <c r="F373">
         <v>260</v>
       </c>
@@ -16949,6 +17205,9 @@
       <c r="D374" t="s">
         <v>20</v>
       </c>
+      <c r="E374">
+        <v>2.7014</v>
+      </c>
       <c r="I374">
         <v>4</v>
       </c>
@@ -16981,6 +17240,9 @@
       <c r="D375" t="s">
         <v>59</v>
       </c>
+      <c r="E375">
+        <v>1.6437999999999999</v>
+      </c>
       <c r="F375">
         <v>110</v>
       </c>
@@ -17025,6 +17287,9 @@
       <c r="D376" t="s">
         <v>71</v>
       </c>
+      <c r="E376">
+        <v>0</v>
+      </c>
       <c r="F376">
         <v>280</v>
       </c>
@@ -17069,6 +17334,9 @@
       <c r="D377" t="s">
         <v>20</v>
       </c>
+      <c r="E377">
+        <v>1.6198999999999999</v>
+      </c>
       <c r="I377">
         <v>3</v>
       </c>
@@ -17101,6 +17369,9 @@
       <c r="D378" t="s">
         <v>59</v>
       </c>
+      <c r="E378">
+        <v>2.8529</v>
+      </c>
       <c r="F378">
         <v>215</v>
       </c>
@@ -17149,7 +17420,7 @@
         <v>71</v>
       </c>
       <c r="E379">
-        <v>0</v>
+        <v>1.3454999999999999</v>
       </c>
       <c r="F379">
         <v>235</v>
@@ -17433,6 +17704,9 @@
       <c r="D385" t="s">
         <v>71</v>
       </c>
+      <c r="E385">
+        <v>0.871</v>
+      </c>
       <c r="F385">
         <v>180</v>
       </c>
@@ -17477,6 +17751,9 @@
       <c r="D386" t="s">
         <v>20</v>
       </c>
+      <c r="E386">
+        <v>3.238</v>
+      </c>
       <c r="I386">
         <v>1</v>
       </c>
@@ -17512,6 +17789,9 @@
       <c r="D387" t="s">
         <v>59</v>
       </c>
+      <c r="E387">
+        <v>1.6012</v>
+      </c>
       <c r="F387">
         <v>95</v>
       </c>
@@ -17606,6 +17886,9 @@
       <c r="D389" t="s">
         <v>20</v>
       </c>
+      <c r="E389">
+        <v>4.6173000000000002</v>
+      </c>
       <c r="I389">
         <v>4</v>
       </c>
@@ -17638,6 +17921,9 @@
       <c r="D390" t="s">
         <v>59</v>
       </c>
+      <c r="E390">
+        <v>4.5079000000000002</v>
+      </c>
       <c r="F390">
         <v>210</v>
       </c>
@@ -17682,6 +17968,9 @@
       <c r="D391" t="s">
         <v>71</v>
       </c>
+      <c r="E391">
+        <v>6.8569000000000004</v>
+      </c>
       <c r="F391">
         <v>310</v>
       </c>
@@ -17923,6 +18212,9 @@
       <c r="D396" t="s">
         <v>59</v>
       </c>
+      <c r="E396">
+        <v>0.91549999999999998</v>
+      </c>
       <c r="F396">
         <v>100</v>
       </c>
@@ -17967,6 +18259,9 @@
       <c r="D397" t="s">
         <v>71</v>
       </c>
+      <c r="E397">
+        <v>2.6625000000000001</v>
+      </c>
       <c r="F397">
         <v>160</v>
       </c>
@@ -18011,6 +18306,9 @@
       <c r="D398" t="s">
         <v>20</v>
       </c>
+      <c r="E398">
+        <v>9.6249000000000002</v>
+      </c>
       <c r="I398">
         <v>3</v>
       </c>
@@ -18043,6 +18341,9 @@
       <c r="D399" t="s">
         <v>59</v>
       </c>
+      <c r="E399">
+        <v>0.2082</v>
+      </c>
       <c r="F399">
         <v>185</v>
       </c>
@@ -18090,6 +18391,9 @@
       <c r="D400" t="s">
         <v>71</v>
       </c>
+      <c r="E400">
+        <v>0.63639999999999997</v>
+      </c>
       <c r="F400">
         <v>185</v>
       </c>
@@ -18169,6 +18473,9 @@
       <c r="D402" t="s">
         <v>59</v>
       </c>
+      <c r="E402">
+        <v>4.6910999999999996</v>
+      </c>
       <c r="F402">
         <v>125</v>
       </c>
@@ -18448,6 +18755,9 @@
       <c r="D408" t="s">
         <v>59</v>
       </c>
+      <c r="E408">
+        <v>1.4538</v>
+      </c>
       <c r="F408">
         <v>240</v>
       </c>
@@ -18498,6 +18808,9 @@
       <c r="D409" t="s">
         <v>71</v>
       </c>
+      <c r="E409">
+        <v>0.44069999999999998</v>
+      </c>
       <c r="F409">
         <v>280</v>
       </c>
@@ -18577,6 +18890,9 @@
       <c r="D411" t="s">
         <v>59</v>
       </c>
+      <c r="E411">
+        <v>1.7303999999999999</v>
+      </c>
       <c r="F411">
         <v>140</v>
       </c>
@@ -18621,6 +18937,9 @@
       <c r="D412" t="s">
         <v>71</v>
       </c>
+      <c r="E412">
+        <v>0.81089999999999995</v>
+      </c>
       <c r="F412">
         <v>325</v>
       </c>
@@ -18665,6 +18984,9 @@
       <c r="D413" t="s">
         <v>20</v>
       </c>
+      <c r="E413">
+        <v>1.9019999999999999</v>
+      </c>
       <c r="I413">
         <v>1</v>
       </c>
@@ -18697,6 +19019,9 @@
       <c r="D414" t="s">
         <v>59</v>
       </c>
+      <c r="E414">
+        <v>1.6714</v>
+      </c>
       <c r="F414">
         <v>180</v>
       </c>
@@ -18741,6 +19066,9 @@
       <c r="D415" t="s">
         <v>71</v>
       </c>
+      <c r="E415">
+        <v>0.59099999999999997</v>
+      </c>
       <c r="F415">
         <v>315</v>
       </c>
@@ -18785,6 +19113,9 @@
       <c r="D416" t="s">
         <v>20</v>
       </c>
+      <c r="E416">
+        <v>0.67400000000000004</v>
+      </c>
       <c r="I416">
         <v>7</v>
       </c>
@@ -18973,6 +19304,9 @@
       <c r="D420" t="s">
         <v>59</v>
       </c>
+      <c r="E420">
+        <v>4.3501000000000003</v>
+      </c>
       <c r="F420">
         <v>215</v>
       </c>
@@ -19017,6 +19351,9 @@
       <c r="D421" t="s">
         <v>71</v>
       </c>
+      <c r="E421">
+        <v>0.98250000000000004</v>
+      </c>
       <c r="F421">
         <v>325</v>
       </c>
@@ -19061,6 +19398,9 @@
       <c r="D422" t="s">
         <v>20</v>
       </c>
+      <c r="E422">
+        <v>0.11169999999999999</v>
+      </c>
       <c r="I422">
         <v>6</v>
       </c>
@@ -19093,6 +19433,9 @@
       <c r="D423" t="s">
         <v>59</v>
       </c>
+      <c r="E423">
+        <v>0.61409999999999998</v>
+      </c>
       <c r="F423">
         <v>160</v>
       </c>
@@ -19137,6 +19480,9 @@
       <c r="D424" t="s">
         <v>71</v>
       </c>
+      <c r="E424">
+        <v>2.5857999999999999</v>
+      </c>
       <c r="F424">
         <v>260</v>
       </c>
@@ -19181,6 +19527,9 @@
       <c r="D425" t="s">
         <v>20</v>
       </c>
+      <c r="E425">
+        <v>2.9508000000000001</v>
+      </c>
       <c r="I425">
         <v>1</v>
       </c>
@@ -19213,6 +19562,9 @@
       <c r="D426" t="s">
         <v>59</v>
       </c>
+      <c r="E426">
+        <v>1.2349000000000001</v>
+      </c>
       <c r="F426">
         <v>225</v>
       </c>
@@ -19260,6 +19612,9 @@
       <c r="D427" t="s">
         <v>71</v>
       </c>
+      <c r="E427">
+        <v>1.8757999999999999</v>
+      </c>
       <c r="F427">
         <v>195</v>
       </c>
@@ -19304,6 +19659,9 @@
       <c r="D428" t="s">
         <v>20</v>
       </c>
+      <c r="E428">
+        <v>2.2010999999999998</v>
+      </c>
       <c r="I428">
         <v>9</v>
       </c>
@@ -19498,6 +19856,9 @@
       <c r="D432" t="s">
         <v>59</v>
       </c>
+      <c r="E432">
+        <v>7.0999999999999994E-2</v>
+      </c>
       <c r="F432">
         <v>120</v>
       </c>
@@ -19542,6 +19903,9 @@
       <c r="D433" t="s">
         <v>71</v>
       </c>
+      <c r="E433">
+        <v>1.9347000000000001</v>
+      </c>
       <c r="F433">
         <v>250</v>
       </c>
@@ -19624,6 +19988,9 @@
       <c r="D435" t="s">
         <v>59</v>
       </c>
+      <c r="E435">
+        <v>2.1408</v>
+      </c>
       <c r="F435">
         <v>155</v>
       </c>
@@ -19668,6 +20035,9 @@
       <c r="D436" t="s">
         <v>71</v>
       </c>
+      <c r="E436">
+        <v>1.4505999999999999</v>
+      </c>
       <c r="F436">
         <v>365</v>
       </c>
@@ -19712,6 +20082,9 @@
       <c r="D437" t="s">
         <v>20</v>
       </c>
+      <c r="E437">
+        <v>1.3611</v>
+      </c>
       <c r="I437">
         <v>4</v>
       </c>
@@ -19744,6 +20117,9 @@
       <c r="D438" t="s">
         <v>59</v>
       </c>
+      <c r="E438">
+        <v>1.1267</v>
+      </c>
       <c r="F438">
         <v>225</v>
       </c>
@@ -19788,6 +20164,9 @@
       <c r="D439" t="s">
         <v>71</v>
       </c>
+      <c r="E439">
+        <v>0.17219999999999999</v>
+      </c>
       <c r="F439">
         <v>310</v>
       </c>
@@ -19832,6 +20211,9 @@
       <c r="D440" t="s">
         <v>20</v>
       </c>
+      <c r="E440">
+        <v>0.99239999999999995</v>
+      </c>
       <c r="I440">
         <v>1</v>
       </c>
@@ -20020,6 +20402,9 @@
       <c r="D444" t="s">
         <v>59</v>
       </c>
+      <c r="E444">
+        <v>2.1819000000000002</v>
+      </c>
       <c r="F444">
         <v>220</v>
       </c>
@@ -20067,6 +20452,9 @@
       <c r="D445" t="s">
         <v>71</v>
       </c>
+      <c r="E445">
+        <v>1.2824</v>
+      </c>
       <c r="F445">
         <v>340</v>
       </c>
@@ -20111,6 +20499,9 @@
       <c r="D446" t="s">
         <v>20</v>
       </c>
+      <c r="E446">
+        <v>0.1353</v>
+      </c>
       <c r="I446">
         <v>2</v>
       </c>
@@ -20143,6 +20534,9 @@
       <c r="D447" t="s">
         <v>59</v>
       </c>
+      <c r="E447">
+        <v>1.3746</v>
+      </c>
       <c r="F447">
         <v>190</v>
       </c>
@@ -20187,6 +20581,9 @@
       <c r="D448" t="s">
         <v>71</v>
       </c>
+      <c r="E448">
+        <v>1.3897999999999999</v>
+      </c>
       <c r="F448">
         <v>245</v>
       </c>
@@ -20266,6 +20663,9 @@
       <c r="D450" t="s">
         <v>59</v>
       </c>
+      <c r="E450">
+        <v>4.7343000000000002</v>
+      </c>
       <c r="F450">
         <v>220</v>
       </c>
@@ -20310,6 +20710,9 @@
       <c r="D451" t="s">
         <v>71</v>
       </c>
+      <c r="E451">
+        <v>1.1369</v>
+      </c>
       <c r="F451">
         <v>425</v>
       </c>
@@ -20601,6 +21004,9 @@
       <c r="D457" t="s">
         <v>71</v>
       </c>
+      <c r="E457">
+        <v>2.0139</v>
+      </c>
       <c r="F457">
         <v>465</v>
       </c>
@@ -20883,6 +21289,9 @@
       <c r="D463" t="s">
         <v>71</v>
       </c>
+      <c r="E463">
+        <v>3.601</v>
+      </c>
       <c r="F463">
         <v>390</v>
       </c>
@@ -21012,6 +21421,9 @@
       <c r="D466" t="s">
         <v>71</v>
       </c>
+      <c r="E466">
+        <v>0.68420000000000003</v>
+      </c>
       <c r="F466">
         <v>305</v>
       </c>
@@ -21138,6 +21550,9 @@
       <c r="D469" t="s">
         <v>71</v>
       </c>
+      <c r="E469">
+        <v>0.85170000000000001</v>
+      </c>
       <c r="F469">
         <v>270</v>
       </c>
@@ -21420,6 +21835,9 @@
       <c r="D475" t="s">
         <v>71</v>
       </c>
+      <c r="E475">
+        <v>0.25130000000000002</v>
+      </c>
       <c r="F475">
         <v>275</v>
       </c>
@@ -21546,6 +21964,9 @@
       <c r="D478" t="s">
         <v>71</v>
       </c>
+      <c r="E478">
+        <v>0.68159999999999998</v>
+      </c>
       <c r="F478">
         <v>245</v>
       </c>
@@ -21957,6 +22378,9 @@
       <c r="D487" t="s">
         <v>71</v>
       </c>
+      <c r="E487">
+        <v>2.7212999999999998</v>
+      </c>
       <c r="F487">
         <v>295</v>
       </c>
@@ -22083,6 +22507,9 @@
       <c r="D490" t="s">
         <v>71</v>
       </c>
+      <c r="E490">
+        <v>1.3665</v>
+      </c>
       <c r="F490">
         <v>270</v>
       </c>
@@ -22209,6 +22636,9 @@
       <c r="D493" t="s">
         <v>71</v>
       </c>
+      <c r="E493">
+        <v>3.0386000000000002</v>
+      </c>
       <c r="F493">
         <v>265</v>
       </c>
@@ -22344,6 +22774,9 @@
       <c r="D496" t="s">
         <v>71</v>
       </c>
+      <c r="E496">
+        <v>0.19259999999999999</v>
+      </c>
       <c r="F496">
         <v>315</v>
       </c>
@@ -22491,6 +22924,9 @@
       <c r="D499" t="s">
         <v>71</v>
       </c>
+      <c r="E499">
+        <v>5.6184000000000003</v>
+      </c>
       <c r="F499">
         <v>355</v>
       </c>
@@ -22617,6 +23053,9 @@
       <c r="D502" t="s">
         <v>71</v>
       </c>
+      <c r="E502">
+        <v>2.0947</v>
+      </c>
       <c r="F502">
         <v>375</v>
       </c>
@@ -22661,6 +23100,9 @@
       <c r="D503" t="s">
         <v>20</v>
       </c>
+      <c r="E503">
+        <v>4.48E-2</v>
+      </c>
       <c r="I503">
         <v>0</v>
       </c>
@@ -22740,6 +23182,9 @@
       <c r="D505" t="s">
         <v>71</v>
       </c>
+      <c r="E505">
+        <v>3.2978999999999998</v>
+      </c>
       <c r="F505">
         <v>145</v>
       </c>
@@ -22771,35 +23216,38 @@
         <v>96</v>
       </c>
     </row>
-    <row r="506" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A506" t="s">
+    <row r="506" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A506" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B506" t="s">
+      <c r="B506" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C506">
+      <c r="C506" s="1">
         <v>17</v>
       </c>
-      <c r="D506" t="s">
-        <v>20</v>
-      </c>
-      <c r="I506">
-        <v>0</v>
-      </c>
-      <c r="K506">
+      <c r="D506" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E506" s="1">
+        <v>0</v>
+      </c>
+      <c r="I506" s="1">
+        <v>0</v>
+      </c>
+      <c r="K506" s="1">
         <v>6</v>
       </c>
-      <c r="L506">
+      <c r="L506" s="1">
         <v>6</v>
       </c>
-      <c r="M506">
-        <v>0</v>
-      </c>
-      <c r="N506">
+      <c r="M506" s="1">
+        <v>0</v>
+      </c>
+      <c r="N506" s="1">
         <v>94</v>
       </c>
-      <c r="U506" t="s">
+      <c r="U506" s="1" t="s">
         <v>97</v>
       </c>
     </row>
@@ -22817,7 +23265,7 @@
         <v>59</v>
       </c>
       <c r="E507">
-        <v>0</v>
+        <v>0.82020000000000004</v>
       </c>
       <c r="F507">
         <v>185</v>
@@ -22872,6 +23320,9 @@
       <c r="D508" t="s">
         <v>71</v>
       </c>
+      <c r="E508">
+        <v>0.52339999999999998</v>
+      </c>
       <c r="F508">
         <v>330</v>
       </c>
@@ -22925,6 +23376,9 @@
       <c r="D509" t="s">
         <v>20</v>
       </c>
+      <c r="E509">
+        <v>0.39860000000000001</v>
+      </c>
       <c r="I509">
         <v>0</v>
       </c>
@@ -23013,6 +23467,9 @@
       <c r="D511" t="s">
         <v>71</v>
       </c>
+      <c r="E511">
+        <v>1.3883000000000001</v>
+      </c>
       <c r="F511">
         <v>385</v>
       </c>
@@ -23057,6 +23514,9 @@
       <c r="D512" t="s">
         <v>20</v>
       </c>
+      <c r="E512">
+        <v>0.23749999999999999</v>
+      </c>
       <c r="I512">
         <v>0</v>
       </c>
@@ -23136,6 +23596,9 @@
       <c r="D514" t="s">
         <v>71</v>
       </c>
+      <c r="E514">
+        <v>3.5251000000000001</v>
+      </c>
       <c r="F514">
         <v>305</v>
       </c>
@@ -23180,6 +23643,9 @@
       <c r="D515" t="s">
         <v>20</v>
       </c>
+      <c r="E515">
+        <v>0.107</v>
+      </c>
       <c r="I515">
         <v>0</v>
       </c>
@@ -23265,6 +23731,9 @@
       <c r="D517" t="s">
         <v>71</v>
       </c>
+      <c r="E517">
+        <v>0.3851</v>
+      </c>
       <c r="F517">
         <v>260</v>
       </c>
@@ -23309,6 +23778,9 @@
       <c r="D518" t="s">
         <v>20</v>
       </c>
+      <c r="E518">
+        <v>0.16470000000000001</v>
+      </c>
       <c r="I518">
         <v>0</v>
       </c>
@@ -23409,6 +23881,9 @@
       <c r="D520" t="s">
         <v>71</v>
       </c>
+      <c r="E520">
+        <v>2.5442</v>
+      </c>
       <c r="F520">
         <v>325</v>
       </c>
@@ -23462,6 +23937,9 @@
       <c r="D521" t="s">
         <v>20</v>
       </c>
+      <c r="E521">
+        <v>1.7835000000000001</v>
+      </c>
       <c r="I521">
         <v>1</v>
       </c>
@@ -23541,6 +24019,9 @@
       <c r="D523" t="s">
         <v>71</v>
       </c>
+      <c r="E523">
+        <v>0.64580000000000004</v>
+      </c>
       <c r="F523">
         <v>280</v>
       </c>
@@ -23585,6 +24066,9 @@
       <c r="D524" t="s">
         <v>20</v>
       </c>
+      <c r="E524">
+        <v>0.81399999999999995</v>
+      </c>
       <c r="I524">
         <v>1</v>
       </c>
@@ -23664,6 +24148,9 @@
       <c r="D526" t="s">
         <v>71</v>
       </c>
+      <c r="E526">
+        <v>2.6099000000000001</v>
+      </c>
       <c r="F526">
         <v>325</v>
       </c>
@@ -23708,6 +24195,9 @@
       <c r="D527" t="s">
         <v>20</v>
       </c>
+      <c r="E527">
+        <v>0.70220000000000005</v>
+      </c>
       <c r="I527">
         <v>1</v>
       </c>
@@ -23787,6 +24277,9 @@
       <c r="D529" t="s">
         <v>71</v>
       </c>
+      <c r="E529">
+        <v>1.5516000000000001</v>
+      </c>
       <c r="F529">
         <v>215</v>
       </c>
@@ -23831,6 +24324,9 @@
       <c r="D530" t="s">
         <v>20</v>
       </c>
+      <c r="E530">
+        <v>0.21329999999999999</v>
+      </c>
       <c r="I530">
         <v>0</v>
       </c>
@@ -23864,7 +24360,7 @@
         <v>59</v>
       </c>
       <c r="E531">
-        <v>0</v>
+        <v>1.7379</v>
       </c>
       <c r="F531">
         <v>130</v>
@@ -23919,6 +24415,9 @@
       <c r="D532" t="s">
         <v>71</v>
       </c>
+      <c r="E532">
+        <v>4.1078999999999999</v>
+      </c>
       <c r="F532">
         <v>280</v>
       </c>
@@ -23975,6 +24474,9 @@
       <c r="D533" t="s">
         <v>20</v>
       </c>
+      <c r="E533">
+        <v>0.46629999999999999</v>
+      </c>
       <c r="I533">
         <v>1</v>
       </c>
@@ -24063,6 +24565,9 @@
       <c r="D535" t="s">
         <v>71</v>
       </c>
+      <c r="E535">
+        <v>2.1894</v>
+      </c>
       <c r="F535">
         <v>185</v>
       </c>
@@ -24110,6 +24615,9 @@
       <c r="D536" t="s">
         <v>20</v>
       </c>
+      <c r="E536">
+        <v>0.30669999999999997</v>
+      </c>
       <c r="I536">
         <v>5</v>
       </c>
@@ -24189,6 +24697,9 @@
       <c r="D538" t="s">
         <v>71</v>
       </c>
+      <c r="E538">
+        <v>1.1962999999999999</v>
+      </c>
       <c r="F538">
         <v>385</v>
       </c>
@@ -24315,6 +24826,9 @@
       <c r="D541" t="s">
         <v>71</v>
       </c>
+      <c r="E541">
+        <v>0.61299999999999999</v>
+      </c>
       <c r="F541">
         <v>500</v>
       </c>
@@ -24359,6 +24873,9 @@
       <c r="D542" t="s">
         <v>20</v>
       </c>
+      <c r="E542">
+        <v>0.43130000000000002</v>
+      </c>
       <c r="I542">
         <v>1</v>
       </c>
@@ -24391,6 +24908,9 @@
       <c r="D543" t="s">
         <v>59</v>
       </c>
+      <c r="E543">
+        <v>1.2222999999999999</v>
+      </c>
       <c r="F543">
         <v>210</v>
       </c>
@@ -24503,6 +25023,9 @@
       <c r="D545" t="s">
         <v>20</v>
       </c>
+      <c r="E545">
+        <v>8.5999999999999993E-2</v>
+      </c>
       <c r="I545">
         <v>3</v>
       </c>
@@ -24544,6 +25067,9 @@
       <c r="D546" t="s">
         <v>59</v>
       </c>
+      <c r="E546">
+        <v>0.77969999999999995</v>
+      </c>
       <c r="F546">
         <v>245</v>
       </c>
@@ -24575,47 +25101,50 @@
         <v>98</v>
       </c>
     </row>
-    <row r="547" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A547" t="s">
+    <row r="547" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A547" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B547" t="s">
+      <c r="B547" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C547">
+      <c r="C547" s="1">
         <v>1</v>
       </c>
-      <c r="D547" t="s">
+      <c r="D547" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F547">
+      <c r="E547" s="1">
+        <v>4.0735000000000001</v>
+      </c>
+      <c r="F547" s="1">
         <v>155</v>
       </c>
-      <c r="G547">
+      <c r="G547" s="1">
         <v>130</v>
       </c>
-      <c r="H547">
+      <c r="H547" s="1">
         <v>130</v>
       </c>
-      <c r="I547">
-        <v>0</v>
-      </c>
-      <c r="J547">
-        <v>0</v>
-      </c>
-      <c r="K547">
+      <c r="I547" s="1">
+        <v>0</v>
+      </c>
+      <c r="J547" s="1">
+        <v>0</v>
+      </c>
+      <c r="K547" s="1">
         <v>23</v>
       </c>
-      <c r="L547">
+      <c r="L547" s="1">
         <v>15</v>
       </c>
-      <c r="M547">
-        <v>0</v>
-      </c>
-      <c r="N547">
+      <c r="M547" s="1">
+        <v>0</v>
+      </c>
+      <c r="N547" s="1">
         <v>85</v>
       </c>
-      <c r="U547" t="s">
+      <c r="U547" s="1" t="s">
         <v>98</v>
       </c>
     </row>
@@ -24632,6 +25161,9 @@
       <c r="D548" t="s">
         <v>20</v>
       </c>
+      <c r="E548">
+        <v>9.69E-2</v>
+      </c>
       <c r="I548">
         <v>0</v>
       </c>
@@ -24664,6 +25196,9 @@
       <c r="D549" t="s">
         <v>59</v>
       </c>
+      <c r="E549">
+        <v>4.36E-2</v>
+      </c>
       <c r="F549">
         <v>215</v>
       </c>
@@ -24717,6 +25252,9 @@
       <c r="D550" t="s">
         <v>71</v>
       </c>
+      <c r="E550">
+        <v>0</v>
+      </c>
       <c r="F550">
         <v>155</v>
       </c>
@@ -24770,6 +25308,9 @@
       <c r="D551" t="s">
         <v>20</v>
       </c>
+      <c r="E551">
+        <v>0.04</v>
+      </c>
       <c r="I551">
         <v>0</v>
       </c>
@@ -24811,6 +25352,9 @@
       <c r="D552" t="s">
         <v>59</v>
       </c>
+      <c r="E552">
+        <v>1.2947</v>
+      </c>
       <c r="F552">
         <v>175</v>
       </c>
@@ -24855,6 +25399,9 @@
       <c r="D553" t="s">
         <v>71</v>
       </c>
+      <c r="E553">
+        <v>0.89129999999999998</v>
+      </c>
       <c r="F553">
         <v>225</v>
       </c>
@@ -24934,6 +25481,9 @@
       <c r="D555" t="s">
         <v>59</v>
       </c>
+      <c r="E555">
+        <v>0.1101</v>
+      </c>
       <c r="F555">
         <v>195</v>
       </c>
@@ -24965,50 +25515,53 @@
         <v>98</v>
       </c>
     </row>
-    <row r="556" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A556" t="s">
+    <row r="556" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A556" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B556" t="s">
+      <c r="B556" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C556">
+      <c r="C556" s="1">
         <v>4</v>
       </c>
-      <c r="D556" t="s">
+      <c r="D556" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F556">
+      <c r="E556" s="1">
+        <v>0.3044</v>
+      </c>
+      <c r="F556" s="1">
         <v>245</v>
       </c>
-      <c r="G556">
+      <c r="G556" s="1">
         <v>175</v>
       </c>
-      <c r="H556">
+      <c r="H556" s="1">
         <v>155</v>
       </c>
-      <c r="I556">
+      <c r="I556" s="1">
         <v>5</v>
       </c>
-      <c r="J556">
-        <v>0</v>
-      </c>
-      <c r="K556">
+      <c r="J556" s="1">
+        <v>0</v>
+      </c>
+      <c r="K556" s="1">
         <v>37</v>
       </c>
-      <c r="L556">
+      <c r="L556" s="1">
         <v>15</v>
       </c>
-      <c r="M556">
-        <v>0</v>
-      </c>
-      <c r="N556">
+      <c r="M556" s="1">
+        <v>0</v>
+      </c>
+      <c r="N556" s="1">
         <v>75</v>
       </c>
-      <c r="O556">
+      <c r="O556" s="1">
         <v>15</v>
       </c>
-      <c r="U556" t="s">
+      <c r="U556" s="1" t="s">
         <v>98</v>
       </c>
     </row>
@@ -25025,6 +25578,9 @@
       <c r="D557" t="s">
         <v>20</v>
       </c>
+      <c r="E557">
+        <v>0.219</v>
+      </c>
       <c r="I557">
         <v>0</v>
       </c>
@@ -25057,6 +25613,9 @@
       <c r="D558" t="s">
         <v>59</v>
       </c>
+      <c r="E558">
+        <v>0.1489</v>
+      </c>
       <c r="F558">
         <v>140</v>
       </c>
@@ -25101,6 +25660,9 @@
       <c r="D559" t="s">
         <v>71</v>
       </c>
+      <c r="E559">
+        <v>0.74960000000000004</v>
+      </c>
       <c r="F559">
         <v>115</v>
       </c>
@@ -25180,6 +25742,9 @@
       <c r="D561" t="s">
         <v>59</v>
       </c>
+      <c r="E561">
+        <v>0.28749999999999998</v>
+      </c>
       <c r="F561">
         <v>140</v>
       </c>
@@ -25236,6 +25801,9 @@
       <c r="D562" t="s">
         <v>71</v>
       </c>
+      <c r="E562">
+        <v>1.0139</v>
+      </c>
       <c r="F562">
         <v>370</v>
       </c>
@@ -25289,6 +25857,9 @@
       <c r="D563" t="s">
         <v>20</v>
       </c>
+      <c r="E563">
+        <v>0.37690000000000001</v>
+      </c>
       <c r="I563">
         <v>0</v>
       </c>
@@ -25330,6 +25901,9 @@
       <c r="D564" t="s">
         <v>59</v>
       </c>
+      <c r="E564">
+        <v>0.72040000000000004</v>
+      </c>
       <c r="F564">
         <v>115</v>
       </c>
@@ -25374,6 +25948,9 @@
       <c r="D565" t="s">
         <v>71</v>
       </c>
+      <c r="E565">
+        <v>0.95760000000000001</v>
+      </c>
       <c r="F565">
         <v>255</v>
       </c>
@@ -25418,6 +25995,9 @@
       <c r="D566" t="s">
         <v>20</v>
       </c>
+      <c r="E566">
+        <v>0</v>
+      </c>
       <c r="I566">
         <v>1</v>
       </c>
@@ -25450,6 +26030,9 @@
       <c r="D567" t="s">
         <v>59</v>
       </c>
+      <c r="E567">
+        <v>2.5926</v>
+      </c>
       <c r="F567">
         <v>75</v>
       </c>
@@ -25494,6 +26077,9 @@
       <c r="D568" t="s">
         <v>71</v>
       </c>
+      <c r="E568">
+        <v>1.1535</v>
+      </c>
       <c r="F568">
         <v>245</v>
       </c>
@@ -25538,6 +26124,9 @@
       <c r="D569" t="s">
         <v>20</v>
       </c>
+      <c r="E569">
+        <v>0.46060000000000001</v>
+      </c>
       <c r="I569">
         <v>0</v>
       </c>
@@ -25570,6 +26159,9 @@
       <c r="D570" t="s">
         <v>59</v>
       </c>
+      <c r="E570">
+        <v>0.35199999999999998</v>
+      </c>
       <c r="F570">
         <v>75</v>
       </c>
@@ -25614,6 +26206,9 @@
       <c r="D571" t="s">
         <v>71</v>
       </c>
+      <c r="E571">
+        <v>0.28689999999999999</v>
+      </c>
       <c r="F571">
         <v>95</v>
       </c>
@@ -25658,6 +26253,9 @@
       <c r="D572" t="s">
         <v>20</v>
       </c>
+      <c r="E572">
+        <v>2.8000000000000001E-2</v>
+      </c>
       <c r="I572">
         <v>1</v>
       </c>
@@ -25690,6 +26288,9 @@
       <c r="D573" t="s">
         <v>59</v>
       </c>
+      <c r="E573">
+        <v>2.0941999999999998</v>
+      </c>
       <c r="F573">
         <v>135</v>
       </c>
@@ -25743,6 +26344,9 @@
       <c r="D574" t="s">
         <v>71</v>
       </c>
+      <c r="E574">
+        <v>0.67310000000000003</v>
+      </c>
       <c r="F574">
         <v>160</v>
       </c>
@@ -25796,6 +26400,9 @@
       <c r="D575" t="s">
         <v>20</v>
       </c>
+      <c r="E575">
+        <v>6.5699999999999995E-2</v>
+      </c>
       <c r="I575">
         <v>0</v>
       </c>
@@ -25837,6 +26444,9 @@
       <c r="D576" t="s">
         <v>59</v>
       </c>
+      <c r="E576">
+        <v>0.95340000000000003</v>
+      </c>
       <c r="F576">
         <v>145</v>
       </c>
@@ -25881,6 +26491,9 @@
       <c r="D577" t="s">
         <v>71</v>
       </c>
+      <c r="E577">
+        <v>0.38090000000000002</v>
+      </c>
       <c r="F577">
         <v>185</v>
       </c>
@@ -25925,6 +26538,9 @@
       <c r="D578" t="s">
         <v>20</v>
       </c>
+      <c r="E578">
+        <v>0.2319</v>
+      </c>
       <c r="I578">
         <v>0</v>
       </c>
@@ -25957,6 +26573,9 @@
       <c r="D579" t="s">
         <v>59</v>
       </c>
+      <c r="E579">
+        <v>0.66139999999999999</v>
+      </c>
       <c r="F579">
         <v>110</v>
       </c>
@@ -26001,6 +26620,9 @@
       <c r="D580" t="s">
         <v>71</v>
       </c>
+      <c r="E580">
+        <v>3.41</v>
+      </c>
       <c r="F580">
         <v>150</v>
       </c>
@@ -26045,6 +26667,9 @@
       <c r="D581" t="s">
         <v>20</v>
       </c>
+      <c r="E581">
+        <v>6.7500000000000004E-2</v>
+      </c>
       <c r="I581">
         <v>0</v>
       </c>
@@ -26077,6 +26702,9 @@
       <c r="D582" t="s">
         <v>59</v>
       </c>
+      <c r="E582">
+        <v>0.29339999999999999</v>
+      </c>
       <c r="F582">
         <v>85</v>
       </c>
@@ -26121,6 +26749,9 @@
       <c r="D583" t="s">
         <v>71</v>
       </c>
+      <c r="E583">
+        <v>1.0711999999999999</v>
+      </c>
       <c r="F583">
         <v>240</v>
       </c>
@@ -26165,6 +26796,9 @@
       <c r="D584" t="s">
         <v>20</v>
       </c>
+      <c r="E584">
+        <v>8.43E-2</v>
+      </c>
       <c r="I584">
         <v>1</v>
       </c>
@@ -26197,6 +26831,9 @@
       <c r="D585" t="s">
         <v>59</v>
       </c>
+      <c r="E585">
+        <v>0.20979999999999999</v>
+      </c>
       <c r="F585">
         <v>135</v>
       </c>
@@ -26253,6 +26890,9 @@
       <c r="D586" t="s">
         <v>71</v>
       </c>
+      <c r="E586">
+        <v>1.6792</v>
+      </c>
       <c r="F586">
         <v>220</v>
       </c>
@@ -26353,6 +26993,9 @@
       <c r="D588" t="s">
         <v>59</v>
       </c>
+      <c r="E588">
+        <v>2.6082000000000001</v>
+      </c>
       <c r="F588">
         <v>75</v>
       </c>
@@ -26397,6 +27040,9 @@
       <c r="D589" t="s">
         <v>71</v>
       </c>
+      <c r="E589">
+        <v>0.98399999999999999</v>
+      </c>
       <c r="F589">
         <v>275</v>
       </c>
@@ -26441,6 +27087,9 @@
       <c r="D590" t="s">
         <v>20</v>
       </c>
+      <c r="E590">
+        <v>0.28939999999999999</v>
+      </c>
       <c r="I590">
         <v>0</v>
       </c>
@@ -26473,6 +27122,9 @@
       <c r="D591" t="s">
         <v>59</v>
       </c>
+      <c r="E591">
+        <v>1.1774</v>
+      </c>
       <c r="F591">
         <v>115</v>
       </c>
@@ -26517,6 +27169,9 @@
       <c r="D592" t="s">
         <v>71</v>
       </c>
+      <c r="E592">
+        <v>0.29609999999999997</v>
+      </c>
       <c r="F592">
         <v>210</v>
       </c>
@@ -26561,6 +27216,9 @@
       <c r="D593" t="s">
         <v>20</v>
       </c>
+      <c r="E593">
+        <v>6.9099999999999995E-2</v>
+      </c>
       <c r="I593">
         <v>1</v>
       </c>
@@ -26593,6 +27251,9 @@
       <c r="D594" t="s">
         <v>59</v>
       </c>
+      <c r="E594">
+        <v>2.3010000000000002</v>
+      </c>
       <c r="F594">
         <v>100</v>
       </c>
@@ -26637,6 +27298,9 @@
       <c r="D595" t="s">
         <v>71</v>
       </c>
+      <c r="E595">
+        <v>1.3754999999999999</v>
+      </c>
       <c r="F595">
         <v>240</v>
       </c>
@@ -26681,6 +27345,9 @@
       <c r="D596" t="s">
         <v>20</v>
       </c>
+      <c r="E596">
+        <v>8.2100000000000006E-2</v>
+      </c>
       <c r="I596">
         <v>0</v>
       </c>
@@ -26713,6 +27380,9 @@
       <c r="D597" t="s">
         <v>59</v>
       </c>
+      <c r="E597">
+        <v>0.39579999999999999</v>
+      </c>
       <c r="F597">
         <v>95</v>
       </c>
@@ -26766,6 +27436,9 @@
       <c r="D598" t="s">
         <v>71</v>
       </c>
+      <c r="E598">
+        <v>0.74119999999999997</v>
+      </c>
       <c r="F598">
         <v>145</v>
       </c>
@@ -26863,6 +27536,9 @@
       <c r="D600" t="s">
         <v>59</v>
       </c>
+      <c r="E600">
+        <v>0.87590000000000001</v>
+      </c>
       <c r="F600">
         <v>85</v>
       </c>
@@ -26907,6 +27583,9 @@
       <c r="D601" t="s">
         <v>71</v>
       </c>
+      <c r="E601">
+        <v>0.81930000000000003</v>
+      </c>
       <c r="F601">
         <v>295</v>
       </c>
@@ -26951,6 +27630,9 @@
       <c r="D602" t="s">
         <v>20</v>
       </c>
+      <c r="E602">
+        <v>4.48E-2</v>
+      </c>
       <c r="I602">
         <v>0</v>
       </c>
@@ -26983,6 +27665,9 @@
       <c r="D603" t="s">
         <v>59</v>
       </c>
+      <c r="E603">
+        <v>2.1173000000000002</v>
+      </c>
       <c r="F603">
         <v>115</v>
       </c>
@@ -27027,6 +27712,9 @@
       <c r="D604" t="s">
         <v>71</v>
       </c>
+      <c r="E604">
+        <v>2.4634999999999998</v>
+      </c>
       <c r="F604">
         <v>420</v>
       </c>
@@ -27106,6 +27794,9 @@
       <c r="D606" t="s">
         <v>59</v>
       </c>
+      <c r="E606">
+        <v>0.57740000000000002</v>
+      </c>
       <c r="F606">
         <v>125</v>
       </c>
@@ -27150,6 +27841,9 @@
       <c r="D607" t="s">
         <v>71</v>
       </c>
+      <c r="E607">
+        <v>1.2936000000000001</v>
+      </c>
       <c r="F607">
         <v>120</v>
       </c>
@@ -27194,6 +27888,9 @@
       <c r="D608" t="s">
         <v>20</v>
       </c>
+      <c r="E608">
+        <v>8.43E-2</v>
+      </c>
       <c r="I608">
         <v>0</v>
       </c>
@@ -27226,6 +27923,9 @@
       <c r="D609" t="s">
         <v>59</v>
       </c>
+      <c r="E609">
+        <v>0.36220000000000002</v>
+      </c>
       <c r="F609">
         <v>105</v>
       </c>
@@ -27270,6 +27970,9 @@
       <c r="D610" t="s">
         <v>71</v>
       </c>
+      <c r="E610">
+        <v>1.5863</v>
+      </c>
       <c r="F610">
         <v>190</v>
       </c>
@@ -27367,6 +28070,9 @@
       <c r="D612" t="s">
         <v>59</v>
       </c>
+      <c r="E612">
+        <v>0.1757</v>
+      </c>
       <c r="F612">
         <v>155</v>
       </c>
@@ -27420,6 +28126,9 @@
       <c r="D613" t="s">
         <v>71</v>
       </c>
+      <c r="E613">
+        <v>2.9641000000000002</v>
+      </c>
       <c r="F613">
         <v>185</v>
       </c>
@@ -27499,6 +28208,9 @@
       <c r="D615" t="s">
         <v>59</v>
       </c>
+      <c r="E615">
+        <v>1.2513000000000001</v>
+      </c>
       <c r="F615">
         <v>100</v>
       </c>
@@ -27543,6 +28255,9 @@
       <c r="D616" t="s">
         <v>71</v>
       </c>
+      <c r="E616">
+        <v>0.47910000000000003</v>
+      </c>
       <c r="F616">
         <v>130</v>
       </c>
@@ -27622,6 +28337,9 @@
       <c r="D618" t="s">
         <v>59</v>
       </c>
+      <c r="E618">
+        <v>0.58450000000000002</v>
+      </c>
       <c r="F618">
         <v>75</v>
       </c>
@@ -27666,6 +28384,9 @@
       <c r="D619" t="s">
         <v>71</v>
       </c>
+      <c r="E619">
+        <v>0.28389999999999999</v>
+      </c>
       <c r="F619">
         <v>75</v>
       </c>
@@ -27710,6 +28431,9 @@
       <c r="D620" t="s">
         <v>20</v>
       </c>
+      <c r="E620">
+        <v>0.21179999999999999</v>
+      </c>
       <c r="I620">
         <v>0</v>
       </c>
@@ -27742,6 +28466,9 @@
       <c r="D621" t="s">
         <v>59</v>
       </c>
+      <c r="E621">
+        <v>0.7399</v>
+      </c>
       <c r="F621">
         <v>85</v>
       </c>
@@ -27795,6 +28522,9 @@
       <c r="D622" t="s">
         <v>71</v>
       </c>
+      <c r="E622">
+        <v>0.71240000000000003</v>
+      </c>
       <c r="F622">
         <v>125</v>
       </c>
@@ -27848,6 +28578,9 @@
       <c r="D623" t="s">
         <v>20</v>
       </c>
+      <c r="E623">
+        <v>0.18190000000000001</v>
+      </c>
       <c r="I623">
         <v>0</v>
       </c>
@@ -27889,6 +28622,9 @@
       <c r="D624" t="s">
         <v>59</v>
       </c>
+      <c r="E624">
+        <v>0.85340000000000005</v>
+      </c>
       <c r="F624">
         <v>75</v>
       </c>
@@ -27933,6 +28669,9 @@
       <c r="D625" t="s">
         <v>71</v>
       </c>
+      <c r="E625">
+        <v>2.1562000000000001</v>
+      </c>
       <c r="F625">
         <v>145</v>
       </c>
@@ -27977,6 +28716,9 @@
       <c r="D626" t="s">
         <v>20</v>
       </c>
+      <c r="E626">
+        <v>9.8199999999999996E-2</v>
+      </c>
       <c r="I626">
         <v>0</v>
       </c>
@@ -28009,6 +28751,9 @@
       <c r="D627" t="s">
         <v>59</v>
       </c>
+      <c r="E627">
+        <v>1.7276</v>
+      </c>
       <c r="F627">
         <v>135</v>
       </c>
@@ -28056,6 +28801,9 @@
       <c r="D628" t="s">
         <v>71</v>
       </c>
+      <c r="E628">
+        <v>0.1588</v>
+      </c>
       <c r="F628">
         <v>160</v>
       </c>
@@ -28100,6 +28848,9 @@
       <c r="D629" t="s">
         <v>20</v>
       </c>
+      <c r="E629">
+        <v>0.19570000000000001</v>
+      </c>
       <c r="I629">
         <v>0</v>
       </c>
@@ -28132,6 +28883,9 @@
       <c r="D630" t="s">
         <v>59</v>
       </c>
+      <c r="E630">
+        <v>0.50319999999999998</v>
+      </c>
       <c r="F630">
         <v>105</v>
       </c>
@@ -28176,6 +28930,9 @@
       <c r="D631" t="s">
         <v>71</v>
       </c>
+      <c r="E631">
+        <v>0.65980000000000005</v>
+      </c>
       <c r="F631">
         <v>170</v>
       </c>
@@ -28223,6 +28980,9 @@
       <c r="D632" t="s">
         <v>20</v>
       </c>
+      <c r="E632">
+        <v>0.1613</v>
+      </c>
       <c r="I632">
         <v>0</v>
       </c>
@@ -28255,6 +29015,9 @@
       <c r="D633" t="s">
         <v>59</v>
       </c>
+      <c r="E633">
+        <v>0</v>
+      </c>
       <c r="F633">
         <v>180</v>
       </c>
@@ -28308,6 +29071,9 @@
       <c r="D634" t="s">
         <v>71</v>
       </c>
+      <c r="E634">
+        <v>0.89070000000000005</v>
+      </c>
       <c r="F634">
         <v>240</v>
       </c>
@@ -28360,6 +29126,9 @@
       </c>
       <c r="D635" t="s">
         <v>20</v>
+      </c>
+      <c r="E635">
+        <v>0.1353</v>
       </c>
       <c r="I635">
         <v>0</v>
@@ -28399,7 +29168,7 @@
   <dimension ref="B1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28411,12 +29180,12 @@
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D2">
-        <v>3.6905999999999999</v>
+        <v>13.398899999999999</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D3">
-        <v>0.64629999999999999</v>
+        <v>1.7682</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -28428,7 +29197,7 @@
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12">
         <f>SUM(D1:D11)</f>
-        <v>4.3369</v>
+        <v>15.1671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
most panoche insects tentative ids
</commit_message>
<xml_diff>
--- a/rdm.gradient.2019.datasheet.xlsx
+++ b/rdm.gradient.2019.datasheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3173" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3179" uniqueCount="101">
   <si>
     <t>Region</t>
   </si>
@@ -651,8 +651,8 @@
   <dimension ref="A1:V635"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A113" sqref="A113:XFD113"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P68" sqref="P68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3592,8 +3592,17 @@
       <c r="N64">
         <v>10</v>
       </c>
+      <c r="R64" t="s">
+        <v>22</v>
+      </c>
+      <c r="S64" t="s">
+        <v>26</v>
+      </c>
+      <c r="T64" t="s">
+        <v>27</v>
+      </c>
       <c r="U64" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.25">
@@ -3627,8 +3636,17 @@
       <c r="N65">
         <v>15</v>
       </c>
+      <c r="R65" t="s">
+        <v>22</v>
+      </c>
+      <c r="S65" t="s">
+        <v>26</v>
+      </c>
+      <c r="T65" t="s">
+        <v>27</v>
+      </c>
       <c r="U65" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
script to clean data
</commit_message>
<xml_diff>
--- a/rdm.gradient.2019.datasheet.xlsx
+++ b/rdm.gradient.2019.datasheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3179" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3181" uniqueCount="102">
   <si>
     <t>Region</t>
   </si>
@@ -330,6 +330,9 @@
   </si>
   <si>
     <t>sum</t>
+  </si>
+  <si>
+    <t>changed C2 O25 veg height from 90 to NA because that is clearly an error</t>
   </si>
 </sst>
 </file>
@@ -650,9 +653,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V635"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P68" sqref="P68"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K295" sqref="K295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3528,7 +3531,7 @@
         <v>3.5543</v>
       </c>
       <c r="I63">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="K63">
         <v>45</v>
@@ -13723,8 +13726,8 @@
       <c r="I295">
         <v>3</v>
       </c>
-      <c r="K295">
-        <v>90</v>
+      <c r="K295" t="s">
+        <v>57</v>
       </c>
       <c r="L295">
         <v>2</v>
@@ -29183,36 +29186,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G12"/>
+  <dimension ref="B1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D2">
         <v>13.398899999999999</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>1.7682</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G5">
         <f>6.8091-0.2927</f>
         <v>6.5164</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12">
         <f>SUM(D1:D11)</f>
         <v>15.1671</v>

</xml_diff>